<commit_message>
[CHANGED] resources/users - changed password to 12345 hashed
</commit_message>
<xml_diff>
--- a/api/src/resources/users.xlsx
+++ b/api/src/resources/users.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moron\Desktop\Henry\GROUP PROJECT\backup\PG-Escuelasconvert\api\src\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moron\Desktop\Henry\GROUP PROJECT\PG-Escuelas\api\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA6AAEA-6D81-40C6-8EB0-67D7635E7366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7EC27D-28DE-4060-A9C6-9AE1B5FFCEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="75">
   <si>
     <t>cuil</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>llll@hotmail.com</t>
+  </si>
+  <si>
+    <t>$2b$10$x0/2y8nbrC55hqKq3jxuBuMt0C1QBXwoUveetxb6U2kuGAxmdWbQ6</t>
   </si>
 </sst>
 </file>
@@ -618,7 +621,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,9 +678,8 @@
       <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="D2">
-        <f>A2</f>
-        <v>20111111111</v>
+      <c r="D2" t="s">
+        <v>74</v>
       </c>
       <c r="E2">
         <v>3511234567</v>
@@ -708,9 +710,8 @@
       <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D13" si="0">A3</f>
-        <v>20111111112</v>
+      <c r="D3" t="s">
+        <v>74</v>
       </c>
       <c r="E3">
         <v>3511278956</v>
@@ -741,9 +742,8 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>20111111113</v>
+      <c r="D4" t="s">
+        <v>74</v>
       </c>
       <c r="E4">
         <v>3511235461</v>
@@ -774,9 +774,8 @@
       <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>20111111114</v>
+      <c r="D5" t="s">
+        <v>74</v>
       </c>
       <c r="E5">
         <v>3513534567</v>
@@ -807,9 +806,8 @@
       <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>20111111115</v>
+      <c r="D6" t="s">
+        <v>74</v>
       </c>
       <c r="E6">
         <v>3511234590</v>
@@ -840,9 +838,8 @@
       <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>20111111116</v>
+      <c r="D7" t="s">
+        <v>74</v>
       </c>
       <c r="E7">
         <v>3511234568</v>
@@ -873,9 +870,8 @@
       <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>20111111117</v>
+      <c r="D8" t="s">
+        <v>74</v>
       </c>
       <c r="E8">
         <v>3511234521</v>
@@ -906,9 +902,8 @@
       <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>20111111118</v>
+      <c r="D9" t="s">
+        <v>74</v>
       </c>
       <c r="E9">
         <v>3511234531</v>
@@ -939,9 +934,8 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>20111111119</v>
+      <c r="D10" t="s">
+        <v>74</v>
       </c>
       <c r="E10">
         <v>3511234580</v>
@@ -972,9 +966,8 @@
       <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>20111111120</v>
+      <c r="D11" t="s">
+        <v>74</v>
       </c>
       <c r="E11">
         <v>3511234595</v>
@@ -1005,9 +998,8 @@
       <c r="C12" t="s">
         <v>25</v>
       </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>20111111121</v>
+      <c r="D12" t="s">
+        <v>74</v>
       </c>
       <c r="E12">
         <v>3511234450</v>
@@ -1038,9 +1030,8 @@
       <c r="C13" t="s">
         <v>26</v>
       </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>20111111122</v>
+      <c r="D13" t="s">
+        <v>74</v>
       </c>
       <c r="E13">
         <v>3511234500</v>

</xml_diff>

<commit_message>
[REFIX] resources/users- password back from hash-> 12345
</commit_message>
<xml_diff>
--- a/api/src/resources/users.xlsx
+++ b/api/src/resources/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moron\Desktop\Henry\GROUP PROJECT\PG-Escuelas\api\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7EC27D-28DE-4060-A9C6-9AE1B5FFCEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726D2BE1-C560-4FF8-B80F-7469A36135C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="74">
   <si>
     <t>cuil</t>
   </si>
@@ -255,9 +255,6 @@
   </si>
   <si>
     <t>llll@hotmail.com</t>
-  </si>
-  <si>
-    <t>$2b$10$x0/2y8nbrC55hqKq3jxuBuMt0C1QBXwoUveetxb6U2kuGAxmdWbQ6</t>
   </si>
 </sst>
 </file>
@@ -329,7 +326,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -337,6 +334,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -621,7 +619,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D2" sqref="D2:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,8 +676,8 @@
       <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
-        <v>74</v>
+      <c r="D2" s="5">
+        <v>12345</v>
       </c>
       <c r="E2">
         <v>3511234567</v>
@@ -710,8 +708,8 @@
       <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
-        <v>74</v>
+      <c r="D3" s="5">
+        <v>12345</v>
       </c>
       <c r="E3">
         <v>3511278956</v>
@@ -742,8 +740,8 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
-        <v>74</v>
+      <c r="D4" s="5">
+        <v>12345</v>
       </c>
       <c r="E4">
         <v>3511235461</v>
@@ -774,8 +772,8 @@
       <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
-        <v>74</v>
+      <c r="D5" s="5">
+        <v>12345</v>
       </c>
       <c r="E5">
         <v>3513534567</v>
@@ -806,8 +804,8 @@
       <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
-        <v>74</v>
+      <c r="D6" s="5">
+        <v>12345</v>
       </c>
       <c r="E6">
         <v>3511234590</v>
@@ -838,8 +836,8 @@
       <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
-        <v>74</v>
+      <c r="D7" s="5">
+        <v>12345</v>
       </c>
       <c r="E7">
         <v>3511234568</v>
@@ -870,8 +868,8 @@
       <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
-        <v>74</v>
+      <c r="D8" s="5">
+        <v>12345</v>
       </c>
       <c r="E8">
         <v>3511234521</v>
@@ -902,8 +900,8 @@
       <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
-        <v>74</v>
+      <c r="D9" s="5">
+        <v>12345</v>
       </c>
       <c r="E9">
         <v>3511234531</v>
@@ -934,8 +932,8 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
-        <v>74</v>
+      <c r="D10" s="5">
+        <v>12345</v>
       </c>
       <c r="E10">
         <v>3511234580</v>
@@ -966,8 +964,8 @@
       <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="D11" t="s">
-        <v>74</v>
+      <c r="D11" s="5">
+        <v>12345</v>
       </c>
       <c r="E11">
         <v>3511234595</v>
@@ -998,8 +996,8 @@
       <c r="C12" t="s">
         <v>25</v>
       </c>
-      <c r="D12" t="s">
-        <v>74</v>
+      <c r="D12" s="5">
+        <v>12345</v>
       </c>
       <c r="E12">
         <v>3511234450</v>
@@ -1030,8 +1028,8 @@
       <c r="C13" t="s">
         <v>26</v>
       </c>
-      <c r="D13" t="s">
-        <v>74</v>
+      <c r="D13" s="5">
+        <v>12345</v>
       </c>
       <c r="E13">
         <v>3511234500</v>

</xml_diff>